<commit_message>
added DE proteins and flatfile
</commit_message>
<xml_diff>
--- a/MScProject/Proteins/8.Krivinko_2018/appi.ajp.2018.17080858.ds004.Table_S6_mapped.xlsx
+++ b/MScProject/Proteins/8.Krivinko_2018/appi.ajp.2018.17080858.ds004.Table_S6_mapped.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\homoe\OneDrive - University of Edinburgh\PROJECT\MScProject\Proteins\8.Krivinko_2018\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_86E9E80E0541D26D43712CC5BAB96FC766C0742E" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{7BB642B4-AC25-4A3D-8060-E14C76906683}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="-17520" windowWidth="24060" windowHeight="15760" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="12" r:id="rId1"/>
@@ -42,8 +48,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Response_1_3.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="Response_1_3.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:zsun28:Downloads:Ding_AD:dataset:Response_1_3.csv" comma="1">
       <textFields count="4">
         <textField type="text"/>
@@ -53,7 +59,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="Response_1_3.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="Response_1_3.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:zsun28:Downloads:Ding_AD:dataset:Response_1_3.csv" comma="1">
       <textFields count="4">
         <textField type="text"/>
@@ -63,7 +69,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="Response_1_3.csv2" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="Response_1_3.csv2" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:zsun28:Downloads:Ding_AD:dataset:Response_1_3.csv" comma="1">
       <textFields count="4">
         <textField type="text"/>
@@ -73,7 +79,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="Response_1_3.csv3" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="Response_1_3.csv3" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:zsun28:Downloads:Ding_AD:dataset:Response_1_3.csv" comma="1">
       <textFields count="4">
         <textField type="text"/>
@@ -83,7 +89,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="Response_1_3.csv4" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="Response_1_3.csv4" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:zsun28:Downloads:Ding_AD:dataset:Response_1_3.csv" comma="1">
       <textFields count="4">
         <textField type="text"/>
@@ -93,7 +99,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="Response_1_3.csv5" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" name="Response_1_3.csv5" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:zsun28:Downloads:Ding_AD:dataset:Response_1_3.csv" comma="1">
       <textFields count="4">
         <textField type="text"/>
@@ -103,7 +109,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="Response_1_3.csv6" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" name="Response_1_3.csv6" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:zsun28:Downloads:Ding_AD:dataset:Response_1_3.csv" comma="1">
       <textFields count="4">
         <textField type="text"/>
@@ -113,7 +119,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="Response_1_3.csv7" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" name="Response_1_3.csv7" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:zsun28:Downloads:Ding_AD:dataset:Response_1_3.csv" comma="1">
       <textFields count="4">
         <textField type="text"/>
@@ -123,7 +129,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="Response_1_3.csv8" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="9" xr16:uid="{00000000-0015-0000-FFFF-FFFF08000000}" name="Response_1_3.csv8" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:zsun28:Downloads:Ding_AD:Response_1_3.csv" comma="1">
       <textFields count="4">
         <textField type="text"/>
@@ -133,7 +139,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="Response_1_3.csv9" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="10" xr16:uid="{00000000-0015-0000-FFFF-FFFF09000000}" name="Response_1_3.csv9" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:zsun28:Downloads:Ding_AD:Response_1_3.csv" comma="1">
       <textFields count="4">
         <textField type="text"/>
@@ -843,7 +849,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="12"/>
@@ -864,6 +870,7 @@
       <sz val="12"/>
       <color indexed="63"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -928,7 +935,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" id="{6BC6088B-74CE-4DEC-9420-BCC8FDB63FA5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BC6088B-74CE-4DEC-9420-BCC8FDB63FA5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1016,43 +1023,43 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Response_1_3" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Response_1_3" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Response_1_3" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Response_1_3" connectionId="8" xr16:uid="{00000000-0016-0000-0A00-000009000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Response_1_3" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Response_1_3" connectionId="2" xr16:uid="{00000000-0016-0000-0200-000001000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Response_1_4" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Response_1_4" connectionId="3" xr16:uid="{00000000-0016-0000-0300-000002000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Response_1_3" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Response_1_3" connectionId="7" xr16:uid="{00000000-0016-0000-0400-000003000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Response_1_3" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Response_1_3" connectionId="6" xr16:uid="{00000000-0016-0000-0500-000004000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Response_1_3" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Response_1_3" connectionId="4" xr16:uid="{00000000-0016-0000-0600-000005000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Response_1_3" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Response_1_3" connectionId="10" xr16:uid="{00000000-0016-0000-0700-000006000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Response_1_3" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Response_1_3" connectionId="5" xr16:uid="{00000000-0016-0000-0800-000007000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Response_1_3" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Response_1_3" connectionId="9" xr16:uid="{00000000-0016-0000-0900-000008000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1376,14 +1383,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.6"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <extLst>
@@ -1395,14 +1401,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D190"/>
   <sheetViews>
     <sheetView topLeftCell="A118" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -4070,7 +4076,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D191">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D191">
     <sortCondition ref="B2:B191"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4084,14 +4090,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -6759,7 +6765,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D190">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D190">
     <sortCondition ref="B2:B190"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6773,17 +6779,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+    <sheetView topLeftCell="A181" workbookViewId="0">
       <selection activeCell="C190" sqref="C190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="34.09765625" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -10589,8 +10596,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <sortState ref="A2:D190">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D190">
     <sortCondition ref="C2:C190"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -10605,14 +10611,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D190"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A37" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -10621,7 +10627,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>55</v>
@@ -10635,7 +10641,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>0.56132800471483901</v>
@@ -10649,7 +10655,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>0.50830009104903195</v>
@@ -10663,7 +10669,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
       <c r="B4">
         <v>0.66516385609806405</v>
@@ -10677,7 +10683,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>214</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <v>0.56855387430451598</v>
@@ -10691,7 +10697,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B6">
         <v>0.414845634301935</v>
@@ -10705,7 +10711,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="B7">
         <v>0.51335242031741901</v>
@@ -10719,7 +10725,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>139</v>
+        <v>65</v>
       </c>
       <c r="B8">
         <v>0.48624444564000002</v>
@@ -10733,7 +10739,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="B9">
         <v>0.51816178599612905</v>
@@ -10747,7 +10753,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>160</v>
+        <v>67</v>
       </c>
       <c r="B10">
         <v>0.47803786392516101</v>
@@ -10761,7 +10767,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="B11">
         <v>0.42502971916774201</v>
@@ -10775,7 +10781,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="B12">
         <v>0.46870156032774202</v>
@@ -10789,7 +10795,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="B13">
         <v>0.46118935697677399</v>
@@ -10803,7 +10809,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
       <c r="B14">
         <v>0.49467577607354801</v>
@@ -10817,7 +10823,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B15">
         <v>0.45004418253032202</v>
@@ -10831,7 +10837,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B16">
         <v>0.43732925098193498</v>
@@ -10845,7 +10851,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B17">
         <v>0.51273842358709598</v>
@@ -10859,7 +10865,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>142</v>
+        <v>75</v>
       </c>
       <c r="B18">
         <v>0.49928165256387103</v>
@@ -10873,7 +10879,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>219</v>
+        <v>76</v>
       </c>
       <c r="B19">
         <v>0.38645723487354799</v>
@@ -10887,7 +10893,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B20">
         <v>0.46805578696387101</v>
@@ -10901,7 +10907,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>208</v>
+        <v>78</v>
       </c>
       <c r="B21">
         <v>0.45346978361677398</v>
@@ -10915,7 +10921,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B22">
         <v>0.448263956145806</v>
@@ -10929,7 +10935,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>154</v>
+        <v>80</v>
       </c>
       <c r="B23">
         <v>0.42616816282451597</v>
@@ -10943,7 +10949,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>150</v>
+        <v>81</v>
       </c>
       <c r="B24">
         <v>0.45491500489806402</v>
@@ -10957,7 +10963,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="B25">
         <v>0.462016624086451</v>
@@ -10971,7 +10977,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
       <c r="B26">
         <v>0.46805419002193499</v>
@@ -10985,7 +10991,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B27">
         <v>0.42418801910451598</v>
@@ -10999,7 +11005,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>164</v>
+        <v>85</v>
       </c>
       <c r="B28">
         <v>0.46863900649677398</v>
@@ -11013,7 +11019,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>147</v>
+        <v>86</v>
       </c>
       <c r="B29">
         <v>0.40379621443871</v>
@@ -11027,7 +11033,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>172</v>
+        <v>87</v>
       </c>
       <c r="B30">
         <v>0.40047036206451597</v>
@@ -11041,7 +11047,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B31">
         <v>0.36078948753935502</v>
@@ -11055,7 +11061,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="B32">
         <v>0.40186980586709697</v>
@@ -11069,7 +11075,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B33">
         <v>0.47337036685677403</v>
@@ -11083,7 +11089,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B34">
         <v>0.44697672997032201</v>
@@ -11097,7 +11103,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>215</v>
+        <v>92</v>
       </c>
       <c r="B35">
         <v>0.45013344269290301</v>
@@ -11111,7 +11117,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="B36">
         <v>0.42315422334193498</v>
@@ -11125,7 +11131,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>166</v>
+        <v>94</v>
       </c>
       <c r="B37">
         <v>0.40567681882451601</v>
@@ -11139,7 +11145,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>211</v>
+        <v>95</v>
       </c>
       <c r="B38">
         <v>0.39768078096903198</v>
@@ -11153,7 +11159,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="B39">
         <v>0.37756055933419302</v>
@@ -11167,7 +11173,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>149</v>
+        <v>97</v>
       </c>
       <c r="B40">
         <v>0.37092445601935498</v>
@@ -11181,7 +11187,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>209</v>
+        <v>98</v>
       </c>
       <c r="B41">
         <v>0.38049877008257998</v>
@@ -11195,7 +11201,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="B42">
         <v>0.40522103450451602</v>
@@ -11209,7 +11215,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>174</v>
+        <v>100</v>
       </c>
       <c r="B43">
         <v>0.37741963586580601</v>
@@ -11223,7 +11229,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>2</v>
+        <v>113</v>
       </c>
       <c r="B44">
         <v>0.42344733930580603</v>
@@ -11237,7 +11243,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="B45">
         <v>0.38267849439741902</v>
@@ -11251,7 +11257,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="B46">
         <v>0.36280869443483799</v>
@@ -11265,7 +11271,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="B47">
         <v>0.40690278072258002</v>
@@ -11279,7 +11285,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>165</v>
+        <v>102</v>
       </c>
       <c r="B48">
         <v>0.37627301705548399</v>
@@ -11293,7 +11299,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="B49">
         <v>0.46600927603483899</v>
@@ -11307,7 +11313,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="B50">
         <v>0.30679882426064498</v>
@@ -11321,7 +11327,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="B51">
         <v>0.42910250236387099</v>
@@ -11335,7 +11341,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="B52">
         <v>0.35915254491999998</v>
@@ -11349,7 +11355,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="B53">
         <v>0.43929497327483902</v>
@@ -11363,7 +11369,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="B54">
         <v>0.37595222635612902</v>
@@ -11377,7 +11383,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B55">
         <v>0.40548259124128999</v>
@@ -11391,7 +11397,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="B56">
         <v>0.36191443265032203</v>
@@ -11405,7 +11411,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="B57">
         <v>0.36634748610451601</v>
@@ -11419,7 +11425,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="B58">
         <v>0.38317807377290303</v>
@@ -11433,7 +11439,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="B59">
         <v>0.36695923709161299</v>
@@ -11447,7 +11453,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
-        <v>162</v>
+        <v>117</v>
       </c>
       <c r="B60">
         <v>0.38501020342193498</v>
@@ -11461,7 +11467,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="B61">
         <v>0.35003304441161298</v>
@@ -11475,7 +11481,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
-        <v>182</v>
+        <v>119</v>
       </c>
       <c r="B62">
         <v>0.33569653937806399</v>
@@ -11489,7 +11495,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="B63">
         <v>0.42441767082064502</v>
@@ -11503,7 +11509,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="B64">
         <v>0.35818855571741898</v>
@@ -11517,7 +11523,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="B65">
         <v>0.31955672811612901</v>
@@ -11531,7 +11537,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="1" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="B66">
         <v>0.34760995337290301</v>
@@ -11545,7 +11551,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="1" t="s">
-        <v>17</v>
+        <v>124</v>
       </c>
       <c r="B67">
         <v>0.35274092148258002</v>
@@ -11559,7 +11565,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="1" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="B68">
         <v>0.33714484127612898</v>
@@ -11573,7 +11579,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="1" t="s">
-        <v>204</v>
+        <v>126</v>
       </c>
       <c r="B69">
         <v>0.30630201840903198</v>
@@ -11587,7 +11593,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="1" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B70">
         <v>0.35779850812903202</v>
@@ -11601,7 +11607,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B71">
         <v>0.36333613972000001</v>
@@ -11615,7 +11621,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="1" t="s">
-        <v>69</v>
+        <v>129</v>
       </c>
       <c r="B72">
         <v>0.342606778508387</v>
@@ -11629,7 +11635,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="1" t="s">
-        <v>7</v>
+        <v>130</v>
       </c>
       <c r="B73">
         <v>0.33829765267612899</v>
@@ -11643,7 +11649,7 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="1" t="s">
-        <v>217</v>
+        <v>131</v>
       </c>
       <c r="B74">
         <v>0.30834298424387102</v>
@@ -11657,7 +11663,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="1" t="s">
-        <v>12</v>
+        <v>132</v>
       </c>
       <c r="B75">
         <v>0.29618148678709699</v>
@@ -11671,7 +11677,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="1" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="B76">
         <v>0.28247668440903201</v>
@@ -11685,7 +11691,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B77">
         <v>0.336221703043871</v>
@@ -11699,7 +11705,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="B78">
         <v>0.38545811332903201</v>
@@ -11713,7 +11719,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="1" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="B79">
         <v>0.32276670043354799</v>
@@ -11727,7 +11733,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="1" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="B80">
         <v>0.34366848165935499</v>
@@ -11741,7 +11747,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B81">
         <v>0.36158736550838699</v>
@@ -11755,7 +11761,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="1" t="s">
-        <v>77</v>
+        <v>139</v>
       </c>
       <c r="B82">
         <v>0.30764991488129001</v>
@@ -11769,7 +11775,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="1" t="s">
-        <v>178</v>
+        <v>140</v>
       </c>
       <c r="B83">
         <v>0.35068418723354799</v>
@@ -11783,7 +11789,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="1" t="s">
-        <v>8</v>
+        <v>141</v>
       </c>
       <c r="B84">
         <v>0.32953539276903199</v>
@@ -11797,7 +11803,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="1" t="s">
-        <v>78</v>
+        <v>142</v>
       </c>
       <c r="B85">
         <v>0.29012677201548398</v>
@@ -11811,7 +11817,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B86">
         <v>0.35419708128774202</v>
@@ -11825,7 +11831,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="1" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
       <c r="B87">
         <v>0.26425100387225797</v>
@@ -11839,7 +11845,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="1" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="B88">
         <v>0.32649874939741902</v>
@@ -11853,7 +11859,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="1" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="B89">
         <v>0.34058013565677397</v>
@@ -11867,7 +11873,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="1" t="s">
-        <v>205</v>
+        <v>147</v>
       </c>
       <c r="B90">
         <v>0.32000318033032199</v>
@@ -11881,7 +11887,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="1" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="B91">
         <v>0.35401631406322598</v>
@@ -11895,7 +11901,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="1" t="s">
-        <v>61</v>
+        <v>149</v>
       </c>
       <c r="B92">
         <v>0.23766839089935499</v>
@@ -11909,7 +11915,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B93">
         <v>0.28255208644645102</v>
@@ -11923,7 +11929,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="1" t="s">
-        <v>107</v>
+        <v>151</v>
       </c>
       <c r="B94">
         <v>0.31686222430838701</v>
@@ -11937,7 +11943,7 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="1" t="s">
-        <v>68</v>
+        <v>152</v>
       </c>
       <c r="B95">
         <v>0.26543691498709698</v>
@@ -11951,7 +11957,7 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="1" t="s">
-        <v>63</v>
+        <v>153</v>
       </c>
       <c r="B96">
         <v>0.33816177191741897</v>
@@ -11965,7 +11971,7 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="1" t="s">
-        <v>22</v>
+        <v>154</v>
       </c>
       <c r="B97">
         <v>0.31442986011741902</v>
@@ -11979,7 +11985,7 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="1" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="B98">
         <v>0.29878760183999997</v>
@@ -11993,7 +11999,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="1" t="s">
-        <v>58</v>
+        <v>156</v>
       </c>
       <c r="B99">
         <v>0.24473382789290299</v>
@@ -12007,7 +12013,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="1" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="B100">
         <v>0.27121239955999998</v>
@@ -12021,7 +12027,7 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="1" t="s">
-        <v>87</v>
+        <v>158</v>
       </c>
       <c r="B101">
         <v>0.32280987907612901</v>
@@ -12035,7 +12041,7 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="1" t="s">
-        <v>119</v>
+        <v>159</v>
       </c>
       <c r="B102">
         <v>0.29240759299096802</v>
@@ -12049,7 +12055,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="1" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="B103">
         <v>0.30394073426580598</v>
@@ -12063,7 +12069,7 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="1" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="B104">
         <v>0.27051437745290302</v>
@@ -12077,7 +12083,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="1" t="s">
-        <v>197</v>
+        <v>162</v>
       </c>
       <c r="B105">
         <v>0.26712441723612901</v>
@@ -12091,7 +12097,7 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="1" t="s">
-        <v>25</v>
+        <v>163</v>
       </c>
       <c r="B106">
         <v>0.27975086201548399</v>
@@ -12105,7 +12111,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="1" t="s">
-        <v>59</v>
+        <v>164</v>
       </c>
       <c r="B107">
         <v>0.223522812077419</v>
@@ -12119,7 +12125,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="1" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="B108">
         <v>0.25250797959354798</v>
@@ -12133,7 +12139,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="1" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="B109">
         <v>0.27743055924258098</v>
@@ -12147,7 +12153,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="1" t="s">
-        <v>206</v>
+        <v>167</v>
       </c>
       <c r="B110">
         <v>0.252897887414193</v>
@@ -12161,7 +12167,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="1" t="s">
-        <v>117</v>
+        <v>168</v>
       </c>
       <c r="B111">
         <v>0.246811803793548</v>
@@ -12175,7 +12181,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="1" t="s">
-        <v>112</v>
+        <v>169</v>
       </c>
       <c r="B112">
         <v>0.298989120107097</v>
@@ -12189,7 +12195,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="1" t="s">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="B113">
         <v>0.27818002512645101</v>
@@ -12203,7 +12209,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="1" t="s">
-        <v>213</v>
+        <v>171</v>
       </c>
       <c r="B114">
         <v>0.25875168867741899</v>
@@ -12217,7 +12223,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="1" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B115">
         <v>0.27248293728387102</v>
@@ -12231,7 +12237,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="1" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="B116">
         <v>0.28218831508387099</v>
@@ -12245,7 +12251,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="1" t="s">
-        <v>97</v>
+        <v>173</v>
       </c>
       <c r="B117">
         <v>0.28555993389935502</v>
@@ -12259,7 +12265,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="1" t="s">
-        <v>24</v>
+        <v>174</v>
       </c>
       <c r="B118">
         <v>0.297263601258064</v>
@@ -12273,7 +12279,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="1" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="B119">
         <v>0.29080210455612898</v>
@@ -12287,7 +12293,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="1" t="s">
-        <v>14</v>
+        <v>177</v>
       </c>
       <c r="B120">
         <v>0.26037860132128998</v>
@@ -12301,7 +12307,7 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="1" t="s">
-        <v>218</v>
+        <v>178</v>
       </c>
       <c r="B121">
         <v>0.228429122922581</v>
@@ -12315,7 +12321,7 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="1" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="B122">
         <v>0.26093771591612902</v>
@@ -12329,7 +12335,7 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B123">
         <v>0.25058673573548401</v>
@@ -12343,7 +12349,7 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="1" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="B124">
         <v>0.23541054095354799</v>
@@ -12357,7 +12363,7 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="1" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B125">
         <v>0.23497726850838699</v>
@@ -12371,7 +12377,7 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="1" t="s">
-        <v>137</v>
+        <v>54</v>
       </c>
       <c r="B126">
         <v>0.28358517462709698</v>
@@ -12385,7 +12391,7 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="1" t="s">
-        <v>98</v>
+        <v>183</v>
       </c>
       <c r="B127">
         <v>0.279557552579355</v>
@@ -12399,7 +12405,7 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="1" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="B128">
         <v>0.25632041688645102</v>
@@ -12413,7 +12419,7 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="1" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B129">
         <v>0.27537738106838699</v>
@@ -12427,7 +12433,7 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="1" t="s">
-        <v>114</v>
+        <v>186</v>
       </c>
       <c r="B130">
         <v>0.23302289758064501</v>
@@ -12441,7 +12447,7 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="1" t="s">
-        <v>88</v>
+        <v>187</v>
       </c>
       <c r="B131">
         <v>-0.27942517748903201</v>
@@ -12455,7 +12461,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B132">
         <v>0.225590868270968</v>
@@ -12469,7 +12475,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="1" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B133">
         <v>0.23221416267871001</v>
@@ -12483,7 +12489,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="1" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="B134">
         <v>0.24496923900258</v>
@@ -12497,7 +12503,7 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="1" t="s">
-        <v>80</v>
+        <v>191</v>
       </c>
       <c r="B135">
         <v>0.29602136719354799</v>
@@ -12511,7 +12517,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B136">
         <v>0.206746887463226</v>
@@ -12525,7 +12531,7 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="1" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="B137">
         <v>0.22168891915612901</v>
@@ -12539,7 +12545,7 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="1" t="s">
-        <v>89</v>
+        <v>194</v>
       </c>
       <c r="B138">
         <v>0.19371212110580599</v>
@@ -12553,7 +12559,7 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="1" t="s">
-        <v>74</v>
+        <v>195</v>
       </c>
       <c r="B139">
         <v>0.25049473142322598</v>
@@ -12567,7 +12573,7 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="1" t="s">
-        <v>116</v>
+        <v>196</v>
       </c>
       <c r="B140">
         <v>0.20622517363741899</v>
@@ -12581,7 +12587,7 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="1" t="s">
-        <v>104</v>
+        <v>197</v>
       </c>
       <c r="B141">
         <v>0.22124883767741901</v>
@@ -12595,7 +12601,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="1" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="B142">
         <v>0.14519154872903201</v>
@@ -12609,7 +12615,7 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="1" t="s">
-        <v>19</v>
+        <v>199</v>
       </c>
       <c r="B143">
         <v>0.230513625827097</v>
@@ -12623,7 +12629,7 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B144">
         <v>0.22120671809548401</v>
@@ -12637,7 +12643,7 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B145">
         <v>0.20013313958451601</v>
@@ -12651,7 +12657,7 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="1" t="s">
-        <v>109</v>
+        <v>202</v>
       </c>
       <c r="B146">
         <v>0.172915764050323</v>
@@ -12665,7 +12671,7 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="1" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="B147">
         <v>0.213576623505806</v>
@@ -12679,7 +12685,7 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="1" t="s">
-        <v>100</v>
+        <v>204</v>
       </c>
       <c r="B148">
         <v>0.23608984560258101</v>
@@ -12693,7 +12699,7 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="1" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B149">
         <v>0.21691749009935499</v>
@@ -12707,7 +12713,7 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="1" t="s">
-        <v>143</v>
+        <v>206</v>
       </c>
       <c r="B150">
         <v>0.193079990632258</v>
@@ -12721,7 +12727,7 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="1" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="B151">
         <v>0.196931296312258</v>
@@ -12735,7 +12741,7 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="1" t="s">
-        <v>171</v>
+        <v>208</v>
       </c>
       <c r="B152">
         <v>0.200881568224516</v>
@@ -12749,7 +12755,7 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="1" t="s">
-        <v>81</v>
+        <v>209</v>
       </c>
       <c r="B153">
         <v>0.178099195660645</v>
@@ -12763,7 +12769,7 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="1" t="s">
-        <v>84</v>
+        <v>210</v>
       </c>
       <c r="B154">
         <v>0.125397559529032</v>
@@ -12777,7 +12783,7 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="1" t="s">
-        <v>4</v>
+        <v>211</v>
       </c>
       <c r="B155">
         <v>0.18804539577806501</v>
@@ -12791,7 +12797,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="1" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="B156">
         <v>-0.18447365341677399</v>
@@ -12805,7 +12811,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="1" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="B157">
         <v>0.13651543532258101</v>
@@ -12819,7 +12825,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="1" t="s">
-        <v>94</v>
+        <v>214</v>
       </c>
       <c r="B158">
         <v>-0.28324870751354803</v>
@@ -12833,7 +12839,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="1" t="s">
-        <v>161</v>
+        <v>215</v>
       </c>
       <c r="B159">
         <v>0.202938964228387</v>
@@ -12847,7 +12853,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="1" t="s">
-        <v>99</v>
+        <v>216</v>
       </c>
       <c r="B160">
         <v>0.132199629789677</v>
@@ -12861,7 +12867,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="1" t="s">
-        <v>115</v>
+        <v>217</v>
       </c>
       <c r="B161">
         <v>-0.18716014402709699</v>
@@ -12875,7 +12881,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B162">
         <v>0.15253311669806399</v>
@@ -12889,7 +12895,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="1" t="s">
-        <v>83</v>
+        <v>219</v>
       </c>
       <c r="B163">
         <v>0.117770443602581</v>
@@ -12903,7 +12909,7 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="1" t="s">
-        <v>168</v>
+        <v>220</v>
       </c>
       <c r="B164">
         <v>0.144186883110968</v>
@@ -12917,7 +12923,7 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="1" t="s">
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="B165">
         <v>-0.16369712905806399</v>
@@ -12931,7 +12937,7 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="1" t="s">
-        <v>207</v>
+        <v>1</v>
       </c>
       <c r="B166">
         <v>0.108269549803871</v>
@@ -12945,7 +12951,7 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B167">
         <v>-0.134891029539355</v>
@@ -12959,7 +12965,7 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="1" t="s">
-        <v>93</v>
+        <v>3</v>
       </c>
       <c r="B168">
         <v>0.10656171248129</v>
@@ -12973,7 +12979,7 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="1" t="s">
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="B169">
         <v>0.115649081295484</v>
@@ -12987,7 +12993,7 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="1" t="s">
-        <v>180</v>
+        <v>5</v>
       </c>
       <c r="B170">
         <v>8.3471556392258006E-2</v>
@@ -13001,7 +13007,7 @@
     </row>
     <row r="171" spans="1:4">
       <c r="A171" s="1" t="s">
-        <v>220</v>
+        <v>6</v>
       </c>
       <c r="B171">
         <v>8.5184492237419293E-2</v>
@@ -13015,7 +13021,7 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172" s="1" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
       <c r="B172">
         <v>9.49751902322577E-2</v>
@@ -13029,7 +13035,7 @@
     </row>
     <row r="173" spans="1:4">
       <c r="A173" s="1" t="s">
-        <v>136</v>
+        <v>8</v>
       </c>
       <c r="B173">
         <v>-9.3840259276128907E-2</v>
@@ -13043,7 +13049,7 @@
     </row>
     <row r="174" spans="1:4">
       <c r="A174" s="1" t="s">
-        <v>177</v>
+        <v>9</v>
       </c>
       <c r="B174">
         <v>5.6014676077419299E-2</v>
@@ -13057,7 +13063,7 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" s="1" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="B175">
         <v>6.5135557080000003E-2</v>
@@ -13071,7 +13077,7 @@
     </row>
     <row r="176" spans="1:4">
       <c r="A176" s="1" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="B176">
         <v>6.4250254161290293E-2</v>
@@ -13085,7 +13091,7 @@
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B177">
         <v>7.8295095959999894E-2</v>
@@ -13099,7 +13105,7 @@
     </row>
     <row r="178" spans="1:4">
       <c r="A178" s="1" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="B178">
         <v>-6.6182384909677802E-2</v>
@@ -13113,7 +13119,7 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179" s="1" t="s">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="B179">
         <v>7.7334044252903203E-2</v>
@@ -13127,7 +13133,7 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="1" t="s">
-        <v>163</v>
+        <v>15</v>
       </c>
       <c r="B180">
         <v>6.8559479601290205E-2</v>
@@ -13141,7 +13147,7 @@
     </row>
     <row r="181" spans="1:4">
       <c r="A181" s="1" t="s">
-        <v>196</v>
+        <v>16</v>
       </c>
       <c r="B181">
         <v>-5.6962303449032199E-2</v>
@@ -13155,7 +13161,7 @@
     </row>
     <row r="182" spans="1:4">
       <c r="A182" s="1" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="B182">
         <v>-6.3095686464516104E-2</v>
@@ -13169,7 +13175,7 @@
     </row>
     <row r="183" spans="1:4">
       <c r="A183" s="1" t="s">
-        <v>192</v>
+        <v>18</v>
       </c>
       <c r="B183">
         <v>-4.4456352363870903E-2</v>
@@ -13183,7 +13189,7 @@
     </row>
     <row r="184" spans="1:4">
       <c r="A184" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B184">
         <v>-3.9519987452903201E-2</v>
@@ -13197,7 +13203,7 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B185">
         <v>3.0115980123871001E-2</v>
@@ -13211,7 +13217,7 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" s="1" t="s">
-        <v>152</v>
+        <v>21</v>
       </c>
       <c r="B186">
         <v>-3.0710389172903401E-2</v>
@@ -13225,7 +13231,7 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" s="1" t="s">
-        <v>158</v>
+        <v>22</v>
       </c>
       <c r="B187">
         <v>3.2650283732903199E-2</v>
@@ -13239,7 +13245,7 @@
     </row>
     <row r="188" spans="1:4">
       <c r="A188" s="1" t="s">
-        <v>212</v>
+        <v>23</v>
       </c>
       <c r="B188">
         <v>1.5919771400000001E-2</v>
@@ -13253,7 +13259,7 @@
     </row>
     <row r="189" spans="1:4">
       <c r="A189" s="1" t="s">
-        <v>129</v>
+        <v>24</v>
       </c>
       <c r="B189">
         <v>-8.2237064064516006E-3</v>
@@ -13267,7 +13273,7 @@
     </row>
     <row r="190" spans="1:4">
       <c r="A190" s="1" t="s">
-        <v>193</v>
+        <v>25</v>
       </c>
       <c r="B190">
         <v>2.9812410632258199E-3</v>
@@ -13280,8 +13286,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D190">
-    <sortCondition ref="C2:C190"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A190">
+    <sortCondition ref="A1:A190"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13294,14 +13300,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D190"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -13310,7 +13316,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>55</v>
@@ -13324,7 +13330,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>-0.45029651588327602</v>
@@ -13338,7 +13344,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>162</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>0.38126480627044101</v>
@@ -13352,7 +13358,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>127</v>
+        <v>61</v>
       </c>
       <c r="B4">
         <v>-0.45024239486215101</v>
@@ -13366,7 +13372,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>218</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <v>-0.302654986138575</v>
@@ -13380,7 +13386,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="B6">
         <v>-0.34027429785781899</v>
@@ -13394,7 +13400,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B7">
         <v>-0.384281061458072</v>
@@ -13408,7 +13414,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>163</v>
+        <v>65</v>
       </c>
       <c r="B8">
         <v>-0.40726317560237102</v>
@@ -13422,7 +13428,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>213</v>
+        <v>66</v>
       </c>
       <c r="B9">
         <v>-0.28975863991821899</v>
@@ -13436,7 +13442,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="B10">
         <v>0.340858236290076</v>
@@ -13450,7 +13456,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B11">
         <v>-0.27276577688099501</v>
@@ -13464,7 +13470,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="B12">
         <v>0.31482741571322798</v>
@@ -13478,7 +13484,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="B13">
         <v>-0.304846756004506</v>
@@ -13492,7 +13498,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B14">
         <v>-0.28450764091917102</v>
@@ -13506,7 +13512,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>125</v>
+        <v>72</v>
       </c>
       <c r="B15">
         <v>-0.29722770756177103</v>
@@ -13520,7 +13526,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B16">
         <v>-0.309815063334198</v>
@@ -13534,7 +13540,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>198</v>
+        <v>74</v>
       </c>
       <c r="B17">
         <v>-0.35561703973282099</v>
@@ -13548,7 +13554,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>159</v>
+        <v>75</v>
       </c>
       <c r="B18">
         <v>-0.44315655722595598</v>
@@ -13562,7 +13568,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>123</v>
+        <v>76</v>
       </c>
       <c r="B19">
         <v>-0.29021603791926798</v>
@@ -13576,7 +13582,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="B20">
         <v>-0.272115429821011</v>
@@ -13590,7 +13596,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="B21">
         <v>-0.33016323472551701</v>
@@ -13604,7 +13610,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="B22">
         <v>-0.264075441687044</v>
@@ -13618,7 +13624,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="B23">
         <v>-0.28270084109124299</v>
@@ -13632,7 +13638,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="B24">
         <v>-0.26024299895020497</v>
@@ -13646,7 +13652,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B25">
         <v>-0.33382894349488501</v>
@@ -13660,7 +13666,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="B26">
         <v>-0.37283926963716701</v>
@@ -13674,7 +13680,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>131</v>
+        <v>84</v>
       </c>
       <c r="B27">
         <v>-0.272443962055336</v>
@@ -13688,7 +13694,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="B28">
         <v>-0.34726639736480702</v>
@@ -13702,7 +13708,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>140</v>
+        <v>86</v>
       </c>
       <c r="B29">
         <v>-0.229037586166663</v>
@@ -13716,7 +13722,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>156</v>
+        <v>87</v>
       </c>
       <c r="B30">
         <v>-0.22373881005370799</v>
@@ -13730,7 +13736,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>158</v>
+        <v>88</v>
       </c>
       <c r="B31">
         <v>-0.35157879666813302</v>
@@ -13744,7 +13750,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B32">
         <v>-0.25454349440134999</v>
@@ -13758,7 +13764,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="B33">
         <v>-0.25378663320504702</v>
@@ -13772,7 +13778,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="B34">
         <v>-0.35285550792449499</v>
@@ -13786,7 +13792,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>168</v>
+        <v>92</v>
       </c>
       <c r="B35">
         <v>-0.30097203288936403</v>
@@ -13800,7 +13806,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>161</v>
+        <v>93</v>
       </c>
       <c r="B36">
         <v>-0.33292241107173498</v>
@@ -13814,7 +13820,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="B37">
         <v>-0.25211772107799402</v>
@@ -13828,7 +13834,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B38">
         <v>-0.24050289537993599</v>
@@ -13842,7 +13848,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>206</v>
+        <v>96</v>
       </c>
       <c r="B39">
         <v>0.197862462854071</v>
@@ -13856,7 +13862,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B40">
         <v>-0.21675557900546999</v>
@@ -13870,7 +13876,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>165</v>
+        <v>98</v>
       </c>
       <c r="B41">
         <v>-0.20517303865773601</v>
@@ -13884,7 +13890,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="B42">
         <v>-0.199571050813031</v>
@@ -13898,7 +13904,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B43">
         <v>-0.20238618390311799</v>
@@ -13912,7 +13918,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B44">
         <v>-0.24691472251714999</v>
@@ -13926,7 +13932,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>1</v>
+        <v>114</v>
       </c>
       <c r="B45">
         <v>-0.22643826268226799</v>
@@ -13940,7 +13946,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B46">
         <v>-0.250191491693459</v>
@@ -13954,7 +13960,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
-        <v>215</v>
+        <v>101</v>
       </c>
       <c r="B47">
         <v>-0.219930653829951</v>
@@ -13968,7 +13974,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B48">
         <v>-0.20071967421363901</v>
@@ -13982,7 +13988,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="B49">
         <v>-0.23762544805403499</v>
@@ -13996,7 +14002,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>201</v>
+        <v>104</v>
       </c>
       <c r="B50">
         <v>-0.21660526332125199</v>
@@ -14010,7 +14016,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="B51">
         <v>-0.18503499706996901</v>
@@ -14024,7 +14030,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>143</v>
+        <v>106</v>
       </c>
       <c r="B52">
         <v>-0.19136973483082401</v>
@@ -14038,7 +14044,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>205</v>
+        <v>107</v>
       </c>
       <c r="B53">
         <v>-0.18923608203251099</v>
@@ -14052,7 +14058,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="B54">
         <v>0.21655822494724</v>
@@ -14066,7 +14072,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
-        <v>157</v>
+        <v>109</v>
       </c>
       <c r="B55">
         <v>-0.17466241168951899</v>
@@ -14080,7 +14086,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B56">
         <v>-0.22583719466610899</v>
@@ -14094,7 +14100,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="B57">
         <v>-0.17063170837625599</v>
@@ -14108,7 +14114,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="B58">
         <v>-0.187372118225728</v>
@@ -14122,7 +14128,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="B59">
         <v>-0.17511196950025401</v>
@@ -14136,7 +14142,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
-        <v>203</v>
+        <v>117</v>
       </c>
       <c r="B60">
         <v>-0.19374070714747199</v>
@@ -14150,7 +14156,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="B61">
         <v>-0.14305996040098501</v>
@@ -14164,7 +14170,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
-        <v>154</v>
+        <v>119</v>
       </c>
       <c r="B62">
         <v>-0.16990254834905999</v>
@@ -14178,7 +14184,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="B63">
         <v>-0.165596753115726</v>
@@ -14192,7 +14198,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="B64">
         <v>-0.165780064855924</v>
@@ -14206,7 +14212,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="B65">
         <v>-0.161334633062309</v>
@@ -14220,7 +14226,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B66">
         <v>-0.235697710588294</v>
@@ -14234,7 +14240,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="1" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="B67">
         <v>-0.16722251826932999</v>
@@ -14248,7 +14254,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B68">
         <v>0.209138035853771</v>
@@ -14262,7 +14268,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="1" t="s">
-        <v>20</v>
+        <v>126</v>
       </c>
       <c r="B69">
         <v>-0.214444994633161</v>
@@ -14276,7 +14282,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="1" t="s">
-        <v>193</v>
+        <v>127</v>
       </c>
       <c r="B70">
         <v>-0.16327563577401499</v>
@@ -14290,7 +14296,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="1" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="B71">
         <v>-0.32838404130175303</v>
@@ -14304,7 +14310,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="B72">
         <v>-0.18108472708492199</v>
@@ -14318,7 +14324,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="1" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="B73">
         <v>-0.20475061955885701</v>
@@ -14332,7 +14338,7 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="1" t="s">
-        <v>171</v>
+        <v>131</v>
       </c>
       <c r="B74">
         <v>0.17405186049707899</v>
@@ -14346,7 +14352,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="1" t="s">
-        <v>5</v>
+        <v>132</v>
       </c>
       <c r="B75">
         <v>-0.15622133225495999</v>
@@ -14360,7 +14366,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="1" t="s">
-        <v>16</v>
+        <v>133</v>
       </c>
       <c r="B76">
         <v>-0.156554973878928</v>
@@ -14374,7 +14380,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="1" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="B77">
         <v>-0.15753285965163399</v>
@@ -14388,7 +14394,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B78">
         <v>-0.15063480139037599</v>
@@ -14402,7 +14408,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="1" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="B79">
         <v>-0.15040229619267201</v>
@@ -14416,7 +14422,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="1" t="s">
-        <v>64</v>
+        <v>137</v>
       </c>
       <c r="B80">
         <v>-0.147361373192156</v>
@@ -14430,7 +14436,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="1" t="s">
-        <v>103</v>
+        <v>138</v>
       </c>
       <c r="B81">
         <v>0.15205257294082999</v>
@@ -14444,7 +14450,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="1" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="B82">
         <v>-0.14934820013182301</v>
@@ -14458,7 +14464,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="1" t="s">
-        <v>182</v>
+        <v>140</v>
       </c>
       <c r="B83">
         <v>-0.138644173078942</v>
@@ -14472,7 +14478,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="1" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="B84">
         <v>-0.15357020973667801</v>
@@ -14486,7 +14492,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B85">
         <v>-0.13609766702324</v>
@@ -14500,7 +14506,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="1" t="s">
-        <v>74</v>
+        <v>143</v>
       </c>
       <c r="B86">
         <v>-0.17934594876683299</v>
@@ -14514,7 +14520,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="1" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="B87">
         <v>-0.14624354110558299</v>
@@ -14528,7 +14534,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="1" t="s">
-        <v>207</v>
+        <v>145</v>
       </c>
       <c r="B88">
         <v>-0.156843588439877</v>
@@ -14542,7 +14548,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="1" t="s">
-        <v>208</v>
+        <v>146</v>
       </c>
       <c r="B89">
         <v>-0.14959663881464799</v>
@@ -14556,7 +14562,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B90">
         <v>0.142940409651863</v>
@@ -14570,7 +14576,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="1" t="s">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="B91">
         <v>-0.14767626023166899</v>
@@ -14584,7 +14590,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="1" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="B92">
         <v>-0.12955453798681399</v>
@@ -14598,7 +14604,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="1" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="B93">
         <v>-0.14212389540224499</v>
@@ -14612,7 +14618,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="1" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="B94">
         <v>-0.135939269523636</v>
@@ -14626,7 +14632,7 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="1" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
       <c r="B95">
         <v>0.14364164561514001</v>
@@ -14640,7 +14646,7 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="1" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
       <c r="B96">
         <v>-0.135169205068399</v>
@@ -14654,7 +14660,7 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="1" t="s">
-        <v>11</v>
+        <v>154</v>
       </c>
       <c r="B97">
         <v>0.138678526406908</v>
@@ -14668,7 +14674,7 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="1" t="s">
-        <v>211</v>
+        <v>155</v>
       </c>
       <c r="B98">
         <v>-0.13432812170556799</v>
@@ -14682,7 +14688,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="1" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="B99">
         <v>-0.12458845752594</v>
@@ -14696,7 +14702,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B100">
         <v>-0.12950503829944801</v>
@@ -14710,7 +14716,7 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="1" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="B101">
         <v>-0.11386447507740501</v>
@@ -14724,7 +14730,7 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="1" t="s">
-        <v>120</v>
+        <v>159</v>
       </c>
       <c r="B102">
         <v>0.13014646455080001</v>
@@ -14738,7 +14744,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="1" t="s">
-        <v>106</v>
+        <v>160</v>
       </c>
       <c r="B103">
         <v>-9.9534954337348699E-2</v>
@@ -14752,7 +14758,7 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="1" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="B104">
         <v>-9.845156058981E-2</v>
@@ -14766,7 +14772,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="1" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="B105">
         <v>-0.12496176149965001</v>
@@ -14780,7 +14786,7 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="1" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="B106">
         <v>9.0250863579328502E-2</v>
@@ -14794,7 +14800,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="1" t="s">
-        <v>7</v>
+        <v>164</v>
       </c>
       <c r="B107">
         <v>-0.11321556916515101</v>
@@ -14808,7 +14814,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="1" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
       <c r="B108">
         <v>-0.116227499625162</v>
@@ -14822,7 +14828,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="1" t="s">
-        <v>214</v>
+        <v>166</v>
       </c>
       <c r="B109">
         <v>-0.12584785774329599</v>
@@ -14836,7 +14842,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="1" t="s">
-        <v>78</v>
+        <v>167</v>
       </c>
       <c r="B110">
         <v>-9.7972558910508503E-2</v>
@@ -14850,7 +14856,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="1" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B111">
         <v>0.114681281830365</v>
@@ -14864,7 +14870,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="1" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="B112">
         <v>-0.114018300429092</v>
@@ -14878,7 +14884,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="1" t="s">
-        <v>61</v>
+        <v>170</v>
       </c>
       <c r="B113">
         <v>-7.9499161008835806E-2</v>
@@ -14892,7 +14898,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="1" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
       <c r="B114">
         <v>-0.10682513471959</v>
@@ -14906,7 +14912,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="1" t="s">
-        <v>87</v>
+        <v>176</v>
       </c>
       <c r="B115">
         <v>0.11697396323717001</v>
@@ -14920,7 +14926,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="1" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="B116">
         <v>-8.4372180385760095E-2</v>
@@ -14934,7 +14940,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="1" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="B117">
         <v>-0.133663580185894</v>
@@ -14948,7 +14954,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="1" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="B118">
         <v>-0.12616542109149401</v>
@@ -14962,7 +14968,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="1" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="B119">
         <v>-9.3235642702471005E-2</v>
@@ -14976,7 +14982,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="1" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="B120">
         <v>-8.2754360407382002E-2</v>
@@ -14990,7 +14996,7 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="1" t="s">
-        <v>212</v>
+        <v>178</v>
       </c>
       <c r="B121">
         <v>0.12160493307520701</v>
@@ -15004,7 +15010,7 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B122">
         <v>0.104623684861138</v>
@@ -15018,7 +15024,7 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="1" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="B123">
         <v>9.1557210324729493E-2</v>
@@ -15032,7 +15038,7 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="1" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B124">
         <v>-8.4015001435037706E-2</v>
@@ -15046,7 +15052,7 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B125">
         <v>8.4987635247216795E-2</v>
@@ -15060,7 +15066,7 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="1" t="s">
-        <v>155</v>
+        <v>54</v>
       </c>
       <c r="B126">
         <v>-7.9390606446391704E-2</v>
@@ -15074,7 +15080,7 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="1" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="B127">
         <v>-9.0054666561498506E-2</v>
@@ -15088,7 +15094,7 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="1" t="s">
-        <v>151</v>
+        <v>184</v>
       </c>
       <c r="B128">
         <v>-8.4498631692439E-2</v>
@@ -15102,7 +15108,7 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="1" t="s">
-        <v>98</v>
+        <v>185</v>
       </c>
       <c r="B129">
         <v>9.3698457831570103E-2</v>
@@ -15116,7 +15122,7 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="1" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="B130">
         <v>8.7355310745366593E-2</v>
@@ -15130,7 +15136,7 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="1" t="s">
-        <v>141</v>
+        <v>187</v>
       </c>
       <c r="B131">
         <v>8.2138916121206301E-2</v>
@@ -15144,7 +15150,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="1" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="B132">
         <v>-7.5336050997443296E-2</v>
@@ -15158,7 +15164,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="1" t="s">
-        <v>69</v>
+        <v>189</v>
       </c>
       <c r="B133">
         <v>-6.9217736242694006E-2</v>
@@ -15172,7 +15178,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="1" t="s">
-        <v>73</v>
+        <v>190</v>
       </c>
       <c r="B134">
         <v>-5.7317855596703098E-2</v>
@@ -15186,7 +15192,7 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="1" t="s">
-        <v>96</v>
+        <v>191</v>
       </c>
       <c r="B135">
         <v>-7.8851593463030306E-2</v>
@@ -15200,7 +15206,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="1" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="B136">
         <v>-8.0877615470221001E-2</v>
@@ -15214,7 +15220,7 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="1" t="s">
-        <v>25</v>
+        <v>193</v>
       </c>
       <c r="B137">
         <v>-6.7732346295850399E-2</v>
@@ -15228,7 +15234,7 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B138">
         <v>-6.6192990545862904E-2</v>
@@ -15242,7 +15248,7 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="1" t="s">
-        <v>67</v>
+        <v>195</v>
       </c>
       <c r="B139">
         <v>7.2262453019830197E-2</v>
@@ -15256,7 +15262,7 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B140">
         <v>-7.2173306840593504E-2</v>
@@ -15270,7 +15276,7 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="1" t="s">
-        <v>22</v>
+        <v>197</v>
       </c>
       <c r="B141">
         <v>-6.9225486440884804E-2</v>
@@ -15284,7 +15290,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B142">
         <v>6.7255783596356006E-2</v>
@@ -15298,7 +15304,7 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B143">
         <v>-5.85423438961159E-2</v>
@@ -15312,7 +15318,7 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="1" t="s">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="B144">
         <v>-5.1888831397634602E-2</v>
@@ -15326,7 +15332,7 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="1" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B145">
         <v>5.5139187773744498E-2</v>
@@ -15340,7 +15346,7 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B146">
         <v>-5.7960244896714398E-2</v>
@@ -15354,7 +15360,7 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="1" t="s">
-        <v>23</v>
+        <v>203</v>
       </c>
       <c r="B147">
         <v>6.2953448961721406E-2</v>
@@ -15368,7 +15374,7 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="1" t="s">
-        <v>89</v>
+        <v>204</v>
       </c>
       <c r="B148">
         <v>5.0464564389935997E-2</v>
@@ -15382,7 +15388,7 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="1" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="B149">
         <v>5.7884721300413999E-2</v>
@@ -15396,7 +15402,7 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="1" t="s">
-        <v>9</v>
+        <v>206</v>
       </c>
       <c r="B150">
         <v>4.4174646112954997E-2</v>
@@ -15410,7 +15416,7 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="1" t="s">
-        <v>135</v>
+        <v>207</v>
       </c>
       <c r="B151">
         <v>5.56705552903725E-2</v>
@@ -15424,7 +15430,7 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="1" t="s">
-        <v>12</v>
+        <v>208</v>
       </c>
       <c r="B152">
         <v>3.9845018240507603E-2</v>
@@ -15438,7 +15444,7 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="1" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
       <c r="B153">
         <v>4.7943888085407102E-2</v>
@@ -15452,7 +15458,7 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="1" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="B154">
         <v>4.4328331729894997E-2</v>
@@ -15466,7 +15472,7 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="1" t="s">
-        <v>192</v>
+        <v>211</v>
       </c>
       <c r="B155">
         <v>-6.7783917298192498E-2</v>
@@ -15480,7 +15486,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="1" t="s">
-        <v>84</v>
+        <v>212</v>
       </c>
       <c r="B156">
         <v>-3.1537069534839701E-2</v>
@@ -15494,7 +15500,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="1" t="s">
-        <v>150</v>
+        <v>213</v>
       </c>
       <c r="B157">
         <v>-4.5272669530379603E-2</v>
@@ -15508,7 +15514,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="1" t="s">
-        <v>183</v>
+        <v>214</v>
       </c>
       <c r="B158">
         <v>-3.0114483889442701E-2</v>
@@ -15522,7 +15528,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="1" t="s">
-        <v>60</v>
+        <v>215</v>
       </c>
       <c r="B159">
         <v>-3.6093073369782201E-2</v>
@@ -15536,7 +15542,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="1" t="s">
-        <v>77</v>
+        <v>216</v>
       </c>
       <c r="B160">
         <v>3.5165091763469797E-2</v>
@@ -15550,7 +15556,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="1" t="s">
-        <v>65</v>
+        <v>217</v>
       </c>
       <c r="B161">
         <v>-3.8818492393309798E-2</v>
@@ -15564,7 +15570,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="1" t="s">
-        <v>8</v>
+        <v>218</v>
       </c>
       <c r="B162">
         <v>-3.5847414011829101E-2</v>
@@ -15578,7 +15584,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="1" t="s">
-        <v>190</v>
+        <v>219</v>
       </c>
       <c r="B163">
         <v>3.6337482294335199E-2</v>
@@ -15592,7 +15598,7 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="1" t="s">
-        <v>137</v>
+        <v>220</v>
       </c>
       <c r="B164">
         <v>3.7803699913700597E-2</v>
@@ -15606,7 +15612,7 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="1" t="s">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="B165">
         <v>3.3792065423028303E-2</v>
@@ -15620,7 +15626,7 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="1" t="s">
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="B166">
         <v>3.1844057846936898E-2</v>
@@ -15634,7 +15640,7 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="1" t="s">
-        <v>187</v>
+        <v>2</v>
       </c>
       <c r="B167">
         <v>3.1203531039956201E-2</v>
@@ -15648,7 +15654,7 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="1" t="s">
-        <v>188</v>
+        <v>3</v>
       </c>
       <c r="B168">
         <v>2.5988304828953299E-2</v>
@@ -15662,7 +15668,7 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B169">
         <v>-3.8736410909608401E-2</v>
@@ -15676,7 +15682,7 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="1" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="B170">
         <v>-2.32323135506202E-2</v>
@@ -15690,7 +15696,7 @@
     </row>
     <row r="171" spans="1:4">
       <c r="A171" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B171">
         <v>2.6993321193773099E-2</v>
@@ -15704,7 +15710,7 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172" s="1" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="B172">
         <v>2.44762886589838E-2</v>
@@ -15718,7 +15724,7 @@
     </row>
     <row r="173" spans="1:4">
       <c r="A173" s="1" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="B173">
         <v>1.7597914264780998E-2</v>
@@ -15732,7 +15738,7 @@
     </row>
     <row r="174" spans="1:4">
       <c r="A174" s="1" t="s">
-        <v>134</v>
+        <v>9</v>
       </c>
       <c r="B174">
         <v>-2.1387167285631201E-2</v>
@@ -15746,7 +15752,7 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" s="1" t="s">
-        <v>185</v>
+        <v>10</v>
       </c>
       <c r="B175">
         <v>-1.97620014492145E-2</v>
@@ -15760,7 +15766,7 @@
     </row>
     <row r="176" spans="1:4">
       <c r="A176" s="1" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="B176">
         <v>-2.1146253377339101E-2</v>
@@ -15774,7 +15780,7 @@
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="1" t="s">
-        <v>219</v>
+        <v>12</v>
       </c>
       <c r="B177">
         <v>-1.5986148993664601E-2</v>
@@ -15788,7 +15794,7 @@
     </row>
     <row r="178" spans="1:4">
       <c r="A178" s="1" t="s">
-        <v>216</v>
+        <v>13</v>
       </c>
       <c r="B178">
         <v>2.1531147455072501E-2</v>
@@ -15802,7 +15808,7 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179" s="1" t="s">
-        <v>217</v>
+        <v>14</v>
       </c>
       <c r="B179">
         <v>1.46715773459481E-2</v>
@@ -15816,7 +15822,7 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="1" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="B180">
         <v>-1.5985634504253901E-2</v>
@@ -15830,7 +15836,7 @@
     </row>
     <row r="181" spans="1:4">
       <c r="A181" s="1" t="s">
-        <v>147</v>
+        <v>16</v>
       </c>
       <c r="B181">
         <v>1.55580531881704E-2</v>
@@ -15844,7 +15850,7 @@
     </row>
     <row r="182" spans="1:4">
       <c r="A182" s="1" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B182">
         <v>-1.6178687174125399E-2</v>
@@ -15858,7 +15864,7 @@
     </row>
     <row r="183" spans="1:4">
       <c r="A183" s="1" t="s">
-        <v>180</v>
+        <v>18</v>
       </c>
       <c r="B183">
         <v>-1.21042661075149E-2</v>
@@ -15872,7 +15878,7 @@
     </row>
     <row r="184" spans="1:4">
       <c r="A184" s="1" t="s">
-        <v>173</v>
+        <v>19</v>
       </c>
       <c r="B184">
         <v>-9.3777289198027202E-3</v>
@@ -15886,7 +15892,7 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B185">
         <v>-7.5633083982598603E-3</v>
@@ -15900,7 +15906,7 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B186">
         <v>4.1565159925804097E-3</v>
@@ -15914,7 +15920,7 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" s="1" t="s">
-        <v>181</v>
+        <v>22</v>
       </c>
       <c r="B187">
         <v>1.82156662866423E-3</v>
@@ -15928,7 +15934,7 @@
     </row>
     <row r="188" spans="1:4">
       <c r="A188" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B188">
         <v>1.24741550542168E-3</v>
@@ -15942,7 +15948,7 @@
     </row>
     <row r="189" spans="1:4">
       <c r="A189" s="1" t="s">
-        <v>172</v>
+        <v>24</v>
       </c>
       <c r="B189">
         <v>-8.3595174904535301E-4</v>
@@ -15956,7 +15962,7 @@
     </row>
     <row r="190" spans="1:4">
       <c r="A190" s="1" t="s">
-        <v>202</v>
+        <v>25</v>
       </c>
       <c r="B190">
         <v>-3.57869595806564E-4</v>
@@ -15969,6 +15975,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A190">
+    <sortCondition ref="A1:A190"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -15980,14 +15989,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D190"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -18655,7 +18664,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A190">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A190">
     <sortCondition ref="A1:A190"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -18669,14 +18678,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -21344,7 +21353,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D190">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D190">
     <sortCondition ref="C2:C190"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -21359,14 +21368,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -24034,7 +24043,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D190">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D190">
     <sortCondition ref="C2:C190"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -24048,14 +24057,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -26723,7 +26732,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D190">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D190">
     <sortCondition ref="C2:C190"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -26738,14 +26747,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D190"/>
   <sheetViews>
     <sheetView topLeftCell="A119" workbookViewId="0">
       <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -29413,7 +29422,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D190">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D190">
     <sortCondition ref="C2:C190"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>